<commit_message>
Add a menu item java processor
</commit_message>
<xml_diff>
--- a/POC/etlap.xlsx
+++ b/POC/etlap.xlsx
@@ -12,14 +12,14 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7740"/>
   </bookViews>
   <sheets>
-    <sheet name="Employee Data" sheetId="1" r:id="rId1"/>
+    <sheet name="HUN" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>Name</t>
   </si>
@@ -27,18 +27,9 @@
     <t>Price</t>
   </si>
   <si>
-    <t>Eloetelek</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
-    <t>Libamaj</t>
-  </si>
-  <si>
-    <t>Hazi libamaj pastetom</t>
-  </si>
-  <si>
     <t>huf</t>
   </si>
   <si>
@@ -51,23 +42,59 @@
     <t>hun</t>
   </si>
   <si>
-    <t>Bruschetta</t>
-  </si>
-  <si>
-    <t>Eredeti Olasz Recept alapjan</t>
+    <t>Hideg eloetelek</t>
+  </si>
+  <si>
+    <t>Tengeri hal trio</t>
+  </si>
+  <si>
+    <t>Atlanti lazactatár, pácolt lazacderék, pácolt tonhal Gundel lazackaviárral</t>
+  </si>
+  <si>
+    <t>Gundel házi készítésű füstölt lazac</t>
+  </si>
+  <si>
+    <t>sült burgonyasalátával</t>
+  </si>
+  <si>
+    <t>Gundel salata 1910</t>
+  </si>
+  <si>
+    <t>(Spárga, paradicsom, uborka, sült paprika, zöldbab, gomba, saláta)</t>
+  </si>
+  <si>
+    <t>Husok</t>
+  </si>
+  <si>
+    <t>Egészben sült borjúbélszín</t>
+  </si>
+  <si>
+    <t>Perigourdine mártással és szarvasgombás felvert burgonyával</t>
+  </si>
+  <si>
+    <t>Bélszínjava Liszt Ferenc módra</t>
+  </si>
+  <si>
+    <t>libamájjal, vadgombákkal és ropogós zöldségekkel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -90,8 +117,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,16 +400,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="69" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -390,58 +418,115 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="C3">
-        <v>1200</v>
+        <v>7500</v>
       </c>
       <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
         <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C4">
-        <v>1600</v>
+        <v>5500</v>
       </c>
       <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" t="s">
-        <v>9</v>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>3900</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <v>13500</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8">
+        <v>13500</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>